<commit_message>
finish class 2 and 3
</commit_message>
<xml_diff>
--- a/apps/matrix-importer/class2.xlsx
+++ b/apps/matrix-importer/class2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryan.zoleta/Projects/toll-ph/apps/matrix-importer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328E6B36-6FD9-3145-93BD-3332487ACD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A7E1B7-D41F-5B4F-900D-9BE5EC99925F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{4EA19FBD-5D92-6444-BD69-1DAF73CA6D21}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{4EA19FBD-5D92-6444-BD69-1DAF73CA6D21}"/>
   </bookViews>
   <sheets>
     <sheet name="TPLEX" sheetId="1" r:id="rId1"/>
@@ -675,9 +675,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1014,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{170A0477-B580-C24C-A663-77C94A36182B}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1293,10 +1294,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946B9BC0-D3F5-9546-A306-F01AB88FB40B}">
-  <dimension ref="A1:AD31"/>
+  <dimension ref="A1:AD67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1398,7 +1399,7 @@
         <v>18</v>
       </c>
       <c r="B2">
-        <v>79</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
@@ -1406,10 +1407,10 @@
         <v>19</v>
       </c>
       <c r="B3">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="C3">
-        <v>79</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -1417,13 +1418,13 @@
         <v>20</v>
       </c>
       <c r="B4">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="C4">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="D4">
-        <v>79</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
@@ -1431,16 +1432,16 @@
         <v>21</v>
       </c>
       <c r="B5">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="C5">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="D5">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="E5">
-        <v>79</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
@@ -1448,19 +1449,19 @@
         <v>22</v>
       </c>
       <c r="B6">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="C6">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="D6">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="E6">
-        <v>79</v>
+        <v>199</v>
       </c>
       <c r="F6">
-        <v>79</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
@@ -1468,22 +1469,22 @@
         <v>23</v>
       </c>
       <c r="B7">
-        <v>90</v>
+        <v>226</v>
       </c>
       <c r="C7">
-        <v>90</v>
+        <v>226</v>
       </c>
       <c r="D7">
-        <v>90</v>
+        <v>226</v>
       </c>
       <c r="E7">
-        <v>90</v>
+        <v>226</v>
       </c>
       <c r="F7">
-        <v>90</v>
+        <v>226</v>
       </c>
       <c r="G7">
-        <v>90</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.2">
@@ -1491,25 +1492,25 @@
         <v>24</v>
       </c>
       <c r="B8">
-        <v>99</v>
+        <v>247</v>
       </c>
       <c r="C8">
-        <v>99</v>
+        <v>247</v>
       </c>
       <c r="D8">
-        <v>99</v>
+        <v>247</v>
       </c>
       <c r="E8">
-        <v>99</v>
+        <v>247</v>
       </c>
       <c r="F8">
-        <v>99</v>
+        <v>247</v>
       </c>
       <c r="G8">
-        <v>99</v>
+        <v>247</v>
       </c>
       <c r="H8">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.2">
@@ -1517,28 +1518,28 @@
         <v>25</v>
       </c>
       <c r="B9">
-        <v>104</v>
+        <v>259</v>
       </c>
       <c r="C9">
-        <v>104</v>
+        <v>259</v>
       </c>
       <c r="D9">
-        <v>104</v>
+        <v>259</v>
       </c>
       <c r="E9">
-        <v>104</v>
+        <v>259</v>
       </c>
       <c r="F9">
-        <v>104</v>
+        <v>259</v>
       </c>
       <c r="G9">
-        <v>104</v>
+        <v>259</v>
       </c>
       <c r="H9">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.2">
@@ -1546,31 +1547,31 @@
         <v>26</v>
       </c>
       <c r="B10">
-        <v>128</v>
+        <v>320</v>
       </c>
       <c r="C10">
-        <v>128</v>
+        <v>320</v>
       </c>
       <c r="D10">
-        <v>128</v>
+        <v>320</v>
       </c>
       <c r="E10">
-        <v>128</v>
+        <v>320</v>
       </c>
       <c r="F10">
-        <v>128</v>
+        <v>320</v>
       </c>
       <c r="G10">
-        <v>128</v>
+        <v>320</v>
       </c>
       <c r="H10">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="I10">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="J10">
-        <v>25</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.2">
@@ -1578,34 +1579,34 @@
         <v>27</v>
       </c>
       <c r="B11">
-        <v>148</v>
+        <v>370</v>
       </c>
       <c r="C11">
-        <v>148</v>
+        <v>370</v>
       </c>
       <c r="D11">
-        <v>148</v>
+        <v>370</v>
       </c>
       <c r="E11">
-        <v>148</v>
+        <v>370</v>
       </c>
       <c r="F11">
-        <v>148</v>
+        <v>370</v>
       </c>
       <c r="G11">
-        <v>148</v>
+        <v>370</v>
       </c>
       <c r="H11">
-        <v>58</v>
+        <v>144</v>
       </c>
       <c r="I11">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="J11">
-        <v>44</v>
+        <v>111</v>
       </c>
       <c r="K11">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.2">
@@ -1613,34 +1614,34 @@
         <v>28</v>
       </c>
       <c r="B12">
-        <v>155</v>
+        <v>387</v>
       </c>
       <c r="C12">
-        <v>155</v>
+        <v>387</v>
       </c>
       <c r="D12">
-        <v>155</v>
+        <v>387</v>
       </c>
       <c r="E12">
-        <v>155</v>
+        <v>387</v>
       </c>
       <c r="F12">
-        <v>155</v>
+        <v>387</v>
       </c>
       <c r="G12">
-        <v>155</v>
+        <v>387</v>
       </c>
       <c r="H12">
-        <v>65</v>
+        <v>162</v>
       </c>
       <c r="I12">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="J12">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="K12">
-        <v>27</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.2">
@@ -1648,37 +1649,37 @@
         <v>29</v>
       </c>
       <c r="B13">
-        <v>190</v>
+        <v>476</v>
       </c>
       <c r="C13">
-        <v>190</v>
+        <v>476</v>
       </c>
       <c r="D13">
-        <v>190</v>
+        <v>476</v>
       </c>
       <c r="E13">
-        <v>190</v>
+        <v>476</v>
       </c>
       <c r="F13">
-        <v>190</v>
+        <v>476</v>
       </c>
       <c r="G13">
-        <v>190</v>
+        <v>476</v>
       </c>
       <c r="H13">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="I13">
-        <v>91</v>
+        <v>229</v>
       </c>
       <c r="J13">
-        <v>87</v>
+        <v>217</v>
       </c>
       <c r="K13">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="L13">
-        <v>35</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.2">
@@ -1686,40 +1687,40 @@
         <v>30</v>
       </c>
       <c r="B14">
-        <v>251</v>
+        <v>627</v>
       </c>
       <c r="C14">
-        <v>251</v>
+        <v>627</v>
       </c>
       <c r="D14">
-        <v>251</v>
+        <v>627</v>
       </c>
       <c r="E14">
-        <v>251</v>
+        <v>627</v>
       </c>
       <c r="F14">
-        <v>251</v>
+        <v>627</v>
       </c>
       <c r="G14">
-        <v>251</v>
+        <v>627</v>
       </c>
       <c r="H14">
-        <v>161</v>
+        <v>402</v>
       </c>
       <c r="I14">
-        <v>152</v>
+        <v>380</v>
       </c>
       <c r="J14">
-        <v>147</v>
+        <v>368</v>
       </c>
       <c r="K14">
-        <v>123</v>
+        <v>307</v>
       </c>
       <c r="L14">
-        <v>96</v>
+        <v>240</v>
       </c>
       <c r="M14">
-        <v>61</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.2">
@@ -1727,43 +1728,43 @@
         <v>31</v>
       </c>
       <c r="B15">
-        <v>297</v>
+        <v>743</v>
       </c>
       <c r="C15">
-        <v>297</v>
+        <v>743</v>
       </c>
       <c r="D15">
-        <v>297</v>
+        <v>743</v>
       </c>
       <c r="E15">
-        <v>297</v>
+        <v>743</v>
       </c>
       <c r="F15">
-        <v>297</v>
+        <v>743</v>
       </c>
       <c r="G15">
-        <v>297</v>
+        <v>743</v>
       </c>
       <c r="H15">
-        <v>207</v>
+        <v>517</v>
       </c>
       <c r="I15">
-        <v>198</v>
+        <v>495</v>
       </c>
       <c r="J15">
-        <v>193</v>
+        <v>483</v>
       </c>
       <c r="K15">
-        <v>169</v>
+        <v>422</v>
       </c>
       <c r="L15">
-        <v>142</v>
+        <v>355</v>
       </c>
       <c r="M15">
-        <v>107</v>
+        <v>267</v>
       </c>
       <c r="N15">
-        <v>46</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.2">
@@ -1771,46 +1772,46 @@
         <v>32</v>
       </c>
       <c r="B16">
-        <v>334</v>
+        <v>834</v>
       </c>
       <c r="C16">
-        <v>334</v>
+        <v>834</v>
       </c>
       <c r="D16">
-        <v>334</v>
+        <v>834</v>
       </c>
       <c r="E16">
-        <v>334</v>
+        <v>834</v>
       </c>
       <c r="F16">
-        <v>334</v>
+        <v>834</v>
       </c>
       <c r="G16">
-        <v>334</v>
+        <v>834</v>
       </c>
       <c r="H16">
-        <v>244</v>
+        <v>609</v>
       </c>
       <c r="I16">
-        <v>235</v>
+        <v>587</v>
       </c>
       <c r="J16">
-        <v>230</v>
+        <v>575</v>
       </c>
       <c r="K16">
-        <v>206</v>
+        <v>514</v>
       </c>
       <c r="L16">
-        <v>179</v>
+        <v>447</v>
       </c>
       <c r="M16">
-        <v>143</v>
+        <v>358</v>
       </c>
       <c r="N16">
-        <v>83</v>
+        <v>207</v>
       </c>
       <c r="O16">
-        <v>37</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -1818,49 +1819,49 @@
         <v>33</v>
       </c>
       <c r="B17">
-        <v>378</v>
+        <v>944</v>
       </c>
       <c r="C17">
-        <v>378</v>
+        <v>944</v>
       </c>
       <c r="D17">
-        <v>378</v>
+        <v>944</v>
       </c>
       <c r="E17">
-        <v>378</v>
+        <v>944</v>
       </c>
       <c r="F17">
-        <v>378</v>
+        <v>944</v>
       </c>
       <c r="G17">
-        <v>378</v>
+        <v>944</v>
       </c>
       <c r="H17">
-        <v>287</v>
+        <v>718</v>
       </c>
       <c r="I17">
-        <v>279</v>
+        <v>696</v>
       </c>
       <c r="J17">
-        <v>274</v>
+        <v>685</v>
       </c>
       <c r="K17">
-        <v>249</v>
+        <v>623</v>
       </c>
       <c r="L17">
-        <v>223</v>
+        <v>557</v>
       </c>
       <c r="M17">
-        <v>187</v>
+        <v>468</v>
       </c>
       <c r="N17">
-        <v>127</v>
+        <v>317</v>
       </c>
       <c r="O17">
-        <v>81</v>
+        <v>201</v>
       </c>
       <c r="P17">
-        <v>44</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
@@ -1868,982 +1869,1117 @@
         <v>34</v>
       </c>
       <c r="B18">
-        <v>388</v>
+        <v>970</v>
       </c>
       <c r="C18">
-        <v>388</v>
+        <v>970</v>
       </c>
       <c r="D18">
-        <v>388</v>
+        <v>970</v>
       </c>
       <c r="E18">
-        <v>388</v>
+        <v>970</v>
       </c>
       <c r="F18">
-        <v>388</v>
+        <v>970</v>
       </c>
       <c r="G18">
-        <v>388</v>
+        <v>970</v>
       </c>
       <c r="H18">
-        <v>298</v>
+        <v>745</v>
       </c>
       <c r="I18">
-        <v>289</v>
+        <v>723</v>
       </c>
       <c r="J18">
-        <v>285</v>
+        <v>711</v>
       </c>
       <c r="K18">
-        <v>260</v>
+        <v>650</v>
       </c>
       <c r="L18">
-        <v>233</v>
+        <v>583</v>
       </c>
       <c r="M18">
-        <v>198</v>
+        <v>494</v>
       </c>
       <c r="N18">
-        <v>137</v>
+        <v>343</v>
       </c>
       <c r="O18">
-        <v>91</v>
+        <v>228</v>
       </c>
       <c r="P18">
-        <v>54</v>
+        <v>136</v>
       </c>
       <c r="Q18">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19">
-        <v>416</v>
-      </c>
-      <c r="C19">
-        <v>416</v>
-      </c>
-      <c r="D19">
-        <v>416</v>
-      </c>
-      <c r="E19">
-        <v>416</v>
-      </c>
-      <c r="F19">
-        <v>416</v>
-      </c>
-      <c r="G19">
-        <v>416</v>
+      <c r="B19" s="2">
+        <v>1039</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1039</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1039</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1039</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1039</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1039</v>
       </c>
       <c r="H19">
-        <v>325</v>
+        <v>814</v>
       </c>
       <c r="I19">
-        <v>317</v>
+        <v>792</v>
       </c>
       <c r="J19">
-        <v>312</v>
+        <v>780</v>
       </c>
       <c r="K19">
-        <v>287</v>
+        <v>719</v>
       </c>
       <c r="L19">
-        <v>261</v>
+        <v>652</v>
       </c>
       <c r="M19">
-        <v>225</v>
+        <v>563</v>
       </c>
       <c r="N19">
-        <v>165</v>
+        <v>412</v>
       </c>
       <c r="O19">
-        <v>119</v>
+        <v>297</v>
       </c>
       <c r="P19">
-        <v>82</v>
+        <v>205</v>
       </c>
       <c r="Q19">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="R19">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>48</v>
       </c>
-      <c r="B20">
-        <v>790</v>
-      </c>
-      <c r="C20">
-        <v>790</v>
-      </c>
-      <c r="D20">
-        <v>790</v>
-      </c>
-      <c r="E20">
-        <v>790</v>
-      </c>
-      <c r="F20">
-        <v>790</v>
-      </c>
-      <c r="G20">
-        <v>790</v>
-      </c>
-      <c r="H20">
-        <v>699</v>
-      </c>
-      <c r="I20">
-        <v>691</v>
-      </c>
-      <c r="J20">
-        <v>686</v>
-      </c>
-      <c r="K20">
-        <v>661</v>
-      </c>
-      <c r="L20">
-        <v>635</v>
-      </c>
-      <c r="M20">
-        <v>599</v>
-      </c>
-      <c r="N20">
-        <v>539</v>
-      </c>
-      <c r="O20">
-        <v>493</v>
+      <c r="B20" s="2">
+        <v>1810</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1810</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1810</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1810</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1810</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1810</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1585</v>
+      </c>
+      <c r="I20" s="2">
+        <v>1563</v>
+      </c>
+      <c r="J20" s="2">
+        <v>1551</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1490</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1423</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1334</v>
+      </c>
+      <c r="N20" s="2">
+        <v>1183</v>
+      </c>
+      <c r="O20" s="2">
+        <v>1068</v>
       </c>
       <c r="P20">
-        <v>456</v>
+        <v>976</v>
       </c>
       <c r="Q20">
-        <v>412</v>
+        <v>866</v>
       </c>
       <c r="R20">
-        <v>401</v>
+        <v>840</v>
       </c>
       <c r="S20">
-        <v>44</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
-      <c r="B21">
-        <v>676</v>
-      </c>
-      <c r="C21">
-        <v>676</v>
-      </c>
-      <c r="D21">
-        <v>676</v>
-      </c>
-      <c r="E21">
-        <v>676</v>
-      </c>
-      <c r="F21">
-        <v>676</v>
-      </c>
-      <c r="G21">
-        <v>676</v>
-      </c>
-      <c r="H21">
-        <v>585</v>
-      </c>
-      <c r="I21">
-        <v>577</v>
-      </c>
-      <c r="J21">
-        <v>572</v>
-      </c>
-      <c r="K21">
-        <v>547</v>
-      </c>
-      <c r="L21">
-        <v>521</v>
-      </c>
-      <c r="M21">
-        <v>485</v>
+      <c r="B21" s="2">
+        <v>1558</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1558</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1558</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1558</v>
+      </c>
+      <c r="F21" s="2">
+        <v>1558</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1558</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1333</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1311</v>
+      </c>
+      <c r="J21" s="2">
+        <v>1299</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1238</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1171</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1082</v>
       </c>
       <c r="N21">
-        <v>425</v>
+        <v>931</v>
       </c>
       <c r="O21">
-        <v>379</v>
+        <v>816</v>
       </c>
       <c r="P21">
-        <v>342</v>
+        <v>724</v>
       </c>
       <c r="Q21">
-        <v>298</v>
+        <v>614</v>
       </c>
       <c r="R21">
-        <v>287</v>
+        <v>588</v>
       </c>
       <c r="S21">
-        <v>114</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>37</v>
       </c>
-      <c r="B22">
-        <v>566</v>
-      </c>
-      <c r="C22">
-        <v>566</v>
-      </c>
-      <c r="D22">
-        <v>566</v>
-      </c>
-      <c r="E22">
-        <v>566</v>
-      </c>
-      <c r="F22">
-        <v>566</v>
-      </c>
-      <c r="G22">
-        <v>566</v>
-      </c>
-      <c r="H22">
-        <v>475</v>
-      </c>
-      <c r="I22">
-        <v>467</v>
-      </c>
-      <c r="J22">
-        <v>462</v>
-      </c>
-      <c r="K22">
-        <v>437</v>
+      <c r="B22" s="2">
+        <v>1339</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1339</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1339</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1339</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1339</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1339</v>
+      </c>
+      <c r="H22" s="2">
+        <v>1114</v>
+      </c>
+      <c r="I22" s="2">
+        <v>1092</v>
+      </c>
+      <c r="J22" s="2">
+        <v>1080</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1019</v>
       </c>
       <c r="L22">
-        <v>411</v>
+        <v>952</v>
       </c>
       <c r="M22">
-        <v>375</v>
+        <v>863</v>
       </c>
       <c r="N22">
-        <v>315</v>
+        <v>712</v>
       </c>
       <c r="O22">
-        <v>269</v>
+        <v>597</v>
       </c>
       <c r="P22">
-        <v>232</v>
+        <v>505</v>
       </c>
       <c r="Q22">
-        <v>188</v>
+        <v>395</v>
       </c>
       <c r="R22">
-        <v>177</v>
+        <v>369</v>
       </c>
       <c r="S22">
-        <v>224</v>
+        <v>470</v>
       </c>
       <c r="T22">
-        <v>109</v>
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>38</v>
       </c>
-      <c r="B23">
-        <v>486</v>
-      </c>
-      <c r="C23">
-        <v>486</v>
-      </c>
-      <c r="D23">
-        <v>486</v>
-      </c>
-      <c r="E23">
-        <v>486</v>
-      </c>
-      <c r="F23">
-        <v>486</v>
-      </c>
-      <c r="G23">
-        <v>486</v>
+      <c r="B23" s="2">
+        <v>1179</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1179</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1179</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1179</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1179</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1179</v>
       </c>
       <c r="H23">
-        <v>395</v>
+        <v>954</v>
       </c>
       <c r="I23">
-        <v>387</v>
+        <v>932</v>
       </c>
       <c r="J23">
-        <v>382</v>
+        <v>920</v>
       </c>
       <c r="K23">
-        <v>357</v>
+        <v>859</v>
       </c>
       <c r="L23">
-        <v>331</v>
+        <v>792</v>
       </c>
       <c r="M23">
-        <v>295</v>
+        <v>703</v>
       </c>
       <c r="N23">
+        <v>552</v>
+      </c>
+      <c r="O23">
+        <v>437</v>
+      </c>
+      <c r="P23">
+        <v>345</v>
+      </c>
+      <c r="Q23">
         <v>235</v>
       </c>
-      <c r="O23">
-        <v>189</v>
-      </c>
-      <c r="P23">
-        <v>152</v>
-      </c>
-      <c r="Q23">
-        <v>108</v>
-      </c>
       <c r="R23">
-        <v>97</v>
+        <v>209</v>
       </c>
       <c r="S23">
-        <v>304</v>
+        <v>630</v>
       </c>
       <c r="T23">
-        <v>190</v>
+        <v>379</v>
       </c>
       <c r="U23">
-        <v>80</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>39</v>
       </c>
-      <c r="B24">
-        <v>426</v>
-      </c>
-      <c r="C24">
-        <v>426</v>
-      </c>
-      <c r="D24">
-        <v>426</v>
-      </c>
-      <c r="E24">
-        <v>426</v>
-      </c>
-      <c r="F24">
-        <v>426</v>
-      </c>
-      <c r="G24">
-        <v>426</v>
+      <c r="B24" s="2">
+        <v>1059</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1059</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1059</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1059</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1059</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1059</v>
       </c>
       <c r="H24">
-        <v>335</v>
+        <v>834</v>
       </c>
       <c r="I24">
-        <v>327</v>
+        <v>812</v>
       </c>
       <c r="J24">
-        <v>322</v>
+        <v>800</v>
       </c>
       <c r="K24">
-        <v>297</v>
+        <v>739</v>
       </c>
       <c r="L24">
-        <v>271</v>
+        <v>672</v>
       </c>
       <c r="M24">
-        <v>235</v>
+        <v>583</v>
       </c>
       <c r="N24">
-        <v>175</v>
+        <v>432</v>
       </c>
       <c r="O24">
-        <v>129</v>
+        <v>317</v>
       </c>
       <c r="P24">
-        <v>92</v>
+        <v>225</v>
       </c>
       <c r="Q24">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="R24">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="S24">
-        <v>364</v>
+        <v>751</v>
       </c>
       <c r="T24">
-        <v>250</v>
+        <v>499</v>
       </c>
       <c r="U24">
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="V24">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>40</v>
       </c>
-      <c r="B25">
-        <v>416</v>
-      </c>
-      <c r="C25">
-        <v>416</v>
-      </c>
-      <c r="D25">
-        <v>416</v>
-      </c>
-      <c r="E25">
-        <v>416</v>
-      </c>
-      <c r="F25">
-        <v>416</v>
-      </c>
-      <c r="G25">
-        <v>416</v>
+      <c r="B25" s="2">
+        <v>1039</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1039</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1039</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1039</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1039</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1039</v>
       </c>
       <c r="H25">
-        <v>325</v>
+        <v>814</v>
       </c>
       <c r="I25">
-        <v>317</v>
+        <v>792</v>
       </c>
       <c r="J25">
-        <v>312</v>
+        <v>780</v>
       </c>
       <c r="K25">
-        <v>287</v>
+        <v>719</v>
       </c>
       <c r="L25">
-        <v>261</v>
+        <v>652</v>
       </c>
       <c r="M25">
-        <v>225</v>
+        <v>563</v>
       </c>
       <c r="N25">
-        <v>165</v>
+        <v>412</v>
       </c>
       <c r="O25">
-        <v>119</v>
+        <v>297</v>
       </c>
       <c r="P25">
-        <v>82</v>
+        <v>205</v>
       </c>
       <c r="Q25">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="R25">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="S25">
-        <v>374</v>
+        <v>771</v>
       </c>
       <c r="T25">
-        <v>260</v>
+        <v>519</v>
       </c>
       <c r="U25">
-        <v>150</v>
+        <v>300</v>
       </c>
       <c r="V25">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="W25">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>41</v>
       </c>
-      <c r="B26">
-        <v>440</v>
-      </c>
-      <c r="C26">
-        <v>440</v>
-      </c>
-      <c r="D26">
-        <v>440</v>
-      </c>
-      <c r="E26">
-        <v>440</v>
-      </c>
-      <c r="F26">
-        <v>440</v>
-      </c>
-      <c r="G26">
-        <v>440</v>
+      <c r="B26" s="2">
+        <v>1087</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1087</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1087</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1087</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1087</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1087</v>
       </c>
       <c r="H26">
-        <v>349</v>
+        <v>862</v>
       </c>
       <c r="I26">
-        <v>341</v>
+        <v>840</v>
       </c>
       <c r="J26">
-        <v>336</v>
+        <v>828</v>
       </c>
       <c r="K26">
-        <v>311</v>
+        <v>767</v>
       </c>
       <c r="L26">
-        <v>285</v>
+        <v>700</v>
       </c>
       <c r="M26">
-        <v>249</v>
+        <v>611</v>
       </c>
       <c r="N26">
-        <v>189</v>
+        <v>460</v>
       </c>
       <c r="O26">
+        <v>345</v>
+      </c>
+      <c r="P26">
+        <v>253</v>
+      </c>
+      <c r="Q26">
         <v>143</v>
       </c>
-      <c r="P26">
-        <v>106</v>
-      </c>
-      <c r="Q26">
-        <v>62</v>
-      </c>
       <c r="R26">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="S26">
-        <v>398</v>
+        <v>819</v>
       </c>
       <c r="T26">
-        <v>284</v>
+        <v>567</v>
       </c>
       <c r="U26">
-        <v>174</v>
+        <v>348</v>
       </c>
       <c r="V26">
-        <v>94</v>
+        <v>188</v>
       </c>
       <c r="W26">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="X26">
-        <v>24</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>42</v>
       </c>
-      <c r="B27">
-        <v>449</v>
-      </c>
-      <c r="C27">
-        <v>449</v>
-      </c>
-      <c r="D27">
-        <v>449</v>
-      </c>
-      <c r="E27">
-        <v>449</v>
-      </c>
-      <c r="F27">
-        <v>449</v>
-      </c>
-      <c r="G27">
-        <v>449</v>
+      <c r="B27" s="2">
+        <v>1105</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1105</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1105</v>
+      </c>
+      <c r="E27" s="2">
+        <v>1105</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1105</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1105</v>
       </c>
       <c r="H27">
-        <v>358</v>
+        <v>880</v>
       </c>
       <c r="I27">
-        <v>350</v>
+        <v>858</v>
       </c>
       <c r="J27">
-        <v>345</v>
+        <v>846</v>
       </c>
       <c r="K27">
-        <v>320</v>
+        <v>785</v>
       </c>
       <c r="L27">
-        <v>294</v>
+        <v>718</v>
       </c>
       <c r="M27">
-        <v>258</v>
+        <v>629</v>
       </c>
       <c r="N27">
-        <v>198</v>
+        <v>478</v>
       </c>
       <c r="O27">
-        <v>152</v>
+        <v>363</v>
       </c>
       <c r="P27">
-        <v>115</v>
+        <v>271</v>
       </c>
       <c r="Q27">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="R27">
-        <v>60</v>
+        <v>135</v>
       </c>
       <c r="S27">
-        <v>407</v>
+        <v>837</v>
       </c>
       <c r="T27">
-        <v>293</v>
+        <v>585</v>
       </c>
       <c r="U27">
-        <v>183</v>
+        <v>366</v>
       </c>
       <c r="V27">
-        <v>103</v>
+        <v>206</v>
       </c>
       <c r="W27">
-        <v>43</v>
+        <v>86</v>
       </c>
       <c r="X27">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="Y27">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B28">
-        <v>488</v>
-      </c>
-      <c r="C28">
-        <v>488</v>
-      </c>
-      <c r="D28">
-        <v>488</v>
-      </c>
-      <c r="E28">
-        <v>488</v>
-      </c>
-      <c r="F28">
-        <v>488</v>
-      </c>
-      <c r="G28">
-        <v>488</v>
+      <c r="B28" s="2">
+        <v>1183</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1183</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1183</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1183</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1183</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1183</v>
       </c>
       <c r="H28">
-        <v>397</v>
+        <v>958</v>
       </c>
       <c r="I28">
-        <v>389</v>
+        <v>936</v>
       </c>
       <c r="J28">
-        <v>384</v>
+        <v>924</v>
       </c>
       <c r="K28">
-        <v>359</v>
+        <v>863</v>
       </c>
       <c r="L28">
-        <v>333</v>
+        <v>796</v>
       </c>
       <c r="M28">
-        <v>297</v>
+        <v>707</v>
       </c>
       <c r="N28">
-        <v>237</v>
+        <v>556</v>
       </c>
       <c r="O28">
-        <v>191</v>
+        <v>441</v>
       </c>
       <c r="P28">
-        <v>154</v>
+        <v>349</v>
       </c>
       <c r="Q28">
-        <v>110</v>
+        <v>239</v>
       </c>
       <c r="R28">
-        <v>99</v>
+        <v>213</v>
       </c>
       <c r="S28">
-        <v>446</v>
+        <v>915</v>
       </c>
       <c r="T28">
-        <v>332</v>
+        <v>663</v>
       </c>
       <c r="U28">
-        <v>222</v>
+        <v>444</v>
       </c>
       <c r="V28">
-        <v>142</v>
+        <v>284</v>
       </c>
       <c r="W28">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="X28">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="Y28">
-        <v>48</v>
+        <v>96</v>
       </c>
       <c r="Z28">
-        <v>39</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>44</v>
       </c>
-      <c r="B29">
-        <v>510</v>
-      </c>
-      <c r="C29">
-        <v>510</v>
-      </c>
-      <c r="D29">
-        <v>510</v>
-      </c>
-      <c r="E29">
-        <v>510</v>
-      </c>
-      <c r="F29">
-        <v>510</v>
-      </c>
-      <c r="G29">
-        <v>510</v>
-      </c>
-      <c r="H29">
-        <v>419</v>
+      <c r="B29" s="2">
+        <v>1227</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1227</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1227</v>
+      </c>
+      <c r="E29" s="2">
+        <v>1227</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1227</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1227</v>
+      </c>
+      <c r="H29" s="2">
+        <v>1002</v>
       </c>
       <c r="I29">
-        <v>411</v>
+        <v>980</v>
       </c>
       <c r="J29">
-        <v>406</v>
+        <v>968</v>
       </c>
       <c r="K29">
-        <v>381</v>
+        <v>907</v>
       </c>
       <c r="L29">
-        <v>355</v>
+        <v>840</v>
       </c>
       <c r="M29">
-        <v>319</v>
+        <v>751</v>
       </c>
       <c r="N29">
-        <v>259</v>
+        <v>600</v>
       </c>
       <c r="O29">
-        <v>213</v>
+        <v>485</v>
       </c>
       <c r="P29">
-        <v>176</v>
+        <v>393</v>
       </c>
       <c r="Q29">
-        <v>132</v>
+        <v>283</v>
       </c>
       <c r="R29">
-        <v>121</v>
+        <v>257</v>
       </c>
       <c r="S29">
-        <v>468</v>
+        <v>958</v>
       </c>
       <c r="T29">
-        <v>353</v>
+        <v>707</v>
       </c>
       <c r="U29">
-        <v>244</v>
+        <v>488</v>
       </c>
       <c r="V29">
-        <v>164</v>
+        <v>328</v>
       </c>
       <c r="W29">
-        <v>104</v>
+        <v>207</v>
       </c>
       <c r="X29">
-        <v>94</v>
+        <v>188</v>
       </c>
       <c r="Y29">
-        <v>70</v>
+        <v>140</v>
       </c>
       <c r="Z29">
-        <v>61</v>
+        <v>122</v>
       </c>
       <c r="AA29">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>45</v>
       </c>
-      <c r="B30">
-        <v>592</v>
-      </c>
-      <c r="C30">
-        <v>592</v>
-      </c>
-      <c r="D30">
-        <v>592</v>
-      </c>
-      <c r="E30">
-        <v>592</v>
-      </c>
-      <c r="F30">
-        <v>592</v>
-      </c>
-      <c r="G30">
-        <v>592</v>
-      </c>
-      <c r="H30">
-        <v>501</v>
-      </c>
-      <c r="I30">
-        <v>493</v>
-      </c>
-      <c r="J30">
-        <v>488</v>
-      </c>
-      <c r="K30">
-        <v>463</v>
-      </c>
-      <c r="L30">
-        <v>437</v>
+      <c r="B30" s="2">
+        <v>1391</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1391</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1391</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1391</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1391</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1391</v>
+      </c>
+      <c r="H30" s="2">
+        <v>1166</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1144</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1132</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1071</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1004</v>
       </c>
       <c r="M30">
-        <v>401</v>
+        <v>915</v>
       </c>
       <c r="N30">
-        <v>341</v>
+        <v>764</v>
       </c>
       <c r="O30">
-        <v>295</v>
+        <v>649</v>
       </c>
       <c r="P30">
-        <v>258</v>
+        <v>557</v>
       </c>
       <c r="Q30">
-        <v>214</v>
+        <v>447</v>
       </c>
       <c r="R30">
-        <v>203</v>
-      </c>
-      <c r="S30">
-        <v>550</v>
+        <v>421</v>
+      </c>
+      <c r="S30" s="2">
+        <v>1123</v>
       </c>
       <c r="T30">
-        <v>436</v>
+        <v>871</v>
       </c>
       <c r="U30">
-        <v>326</v>
+        <v>652</v>
       </c>
       <c r="V30">
-        <v>246</v>
+        <v>492</v>
       </c>
       <c r="W30">
-        <v>186</v>
+        <v>372</v>
       </c>
       <c r="X30">
-        <v>176</v>
+        <v>352</v>
       </c>
       <c r="Y30">
-        <v>152</v>
+        <v>304</v>
       </c>
       <c r="Z30">
-        <v>143</v>
+        <v>286</v>
       </c>
       <c r="AA30">
-        <v>104</v>
+        <v>208</v>
       </c>
       <c r="AB30">
-        <v>82</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>46</v>
       </c>
-      <c r="B31">
-        <v>621</v>
-      </c>
-      <c r="C31">
-        <v>621</v>
-      </c>
-      <c r="D31">
-        <v>621</v>
-      </c>
-      <c r="E31">
-        <v>621</v>
-      </c>
-      <c r="F31">
-        <v>621</v>
-      </c>
-      <c r="G31">
-        <v>621</v>
-      </c>
-      <c r="H31">
-        <v>530</v>
-      </c>
-      <c r="I31">
-        <v>522</v>
-      </c>
-      <c r="J31">
-        <v>517</v>
-      </c>
-      <c r="K31">
-        <v>492</v>
-      </c>
-      <c r="L31">
-        <v>466</v>
+      <c r="B31" s="2">
+        <v>1448</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1448</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1448</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1448</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1448</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1448</v>
+      </c>
+      <c r="H31" s="2">
+        <v>1223</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1201</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1189</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1128</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1061</v>
       </c>
       <c r="M31">
-        <v>430</v>
+        <v>972</v>
       </c>
       <c r="N31">
-        <v>370</v>
+        <v>821</v>
       </c>
       <c r="O31">
-        <v>324</v>
+        <v>706</v>
       </c>
       <c r="P31">
-        <v>287</v>
+        <v>614</v>
       </c>
       <c r="Q31">
-        <v>243</v>
+        <v>504</v>
       </c>
       <c r="R31">
-        <v>232</v>
-      </c>
-      <c r="S31">
-        <v>578</v>
+        <v>478</v>
+      </c>
+      <c r="S31" s="2">
+        <v>1180</v>
       </c>
       <c r="T31">
-        <v>464</v>
+        <v>928</v>
       </c>
       <c r="U31">
-        <v>355</v>
+        <v>709</v>
       </c>
       <c r="V31">
-        <v>275</v>
+        <v>549</v>
       </c>
       <c r="W31">
-        <v>214</v>
+        <v>429</v>
       </c>
       <c r="X31">
-        <v>205</v>
+        <v>409</v>
       </c>
       <c r="Y31">
-        <v>181</v>
+        <v>361</v>
       </c>
       <c r="Z31">
-        <v>172</v>
+        <v>343</v>
       </c>
       <c r="AA31">
-        <v>133</v>
+        <v>265</v>
       </c>
       <c r="AB31">
-        <v>111</v>
+        <v>222</v>
       </c>
       <c r="AC31">
-        <v>29</v>
-      </c>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+    </row>
+    <row r="56" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+      <c r="O56" s="2"/>
+    </row>
+    <row r="57" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+    </row>
+    <row r="58" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+    </row>
+    <row r="59" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+    </row>
+    <row r="63" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+    </row>
+    <row r="64" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+    </row>
+    <row r="65" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+      <c r="S66" s="2"/>
+    </row>
+    <row r="67" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="2"/>
+      <c r="J67" s="2"/>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+      <c r="S67" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3020,8 +3156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2434ACF-B3FC-E74E-8884-182839C01BCF}">
   <dimension ref="A1:V31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D10:D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>